<commit_message>
Update translation + Update picture
</commit_message>
<xml_diff>
--- a/doc/Translation-Therapy-Hessen.xlsx
+++ b/doc/Translation-Therapy-Hessen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Trunk\Samples\TherapyHessen\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projects\Trunk\trnfrt.github.io\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A8C636-316A-4347-B5D5-DAC5CFAF014E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9097FB9C-8FF5-40BE-87A5-468F333EEBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -723,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -754,10 +754,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -976,12 +975,12 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="28.44140625" customWidth="1"/>
@@ -1611,7 +1610,7 @@
         <v>$("[data-lang=child_list_item_14]").text(language.child_list_item_14);</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>141</v>
       </c>
@@ -2338,7 +2337,7 @@
       <c r="A59" t="s">
         <v>185</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B59" s="17" t="s">
         <v>188</v>
       </c>
       <c r="C59" s="13" t="s">
@@ -2375,7 +2374,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>

</xml_diff>